<commit_message>
extra results are added
</commit_message>
<xml_diff>
--- a/Processor/Manufacturing output chart1.xlsx
+++ b/Processor/Manufacturing output chart1.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -36,19 +36,31 @@
     <t>Manufacturing Output Data</t>
   </si>
   <si>
-    <t>GPU No Shuffling</t>
-  </si>
-  <si>
-    <t>GPU With Shuffling</t>
-  </si>
-  <si>
     <t>Lowest Validation Error</t>
   </si>
   <si>
-    <t>CPU No Shuffling</t>
+    <t>HiddenLayer_1_Nodes_450_LearningRate_10_3_Shuffle_True</t>
   </si>
   <si>
-    <t>CPU With Shuffling</t>
+    <t>HiddenLayer_1_Nodes_450_LearningRate_10_3_ShuffleTrue_OneSet</t>
+  </si>
+  <si>
+    <t>hiddenLayer_1_Nodes_250_LearningRate_10_3_Shuffle_False</t>
+  </si>
+  <si>
+    <t>shuffling</t>
+  </si>
+  <si>
+    <t>HiddenLayer_1_Nodes_250_LearningRate_10_3_Suffling_True</t>
+  </si>
+  <si>
+    <t>inc nodes</t>
+  </si>
+  <si>
+    <t>one set</t>
+  </si>
+  <si>
+    <t>Change</t>
   </si>
 </sst>
 </file>
@@ -146,7 +158,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -160,6 +172,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -237,66 +252,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:effectLst/>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US">
-                <a:latin typeface="+mj-lt"/>
-              </a:rPr>
-              <a:t>COMPONENTS COMPLETED</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -321,10 +277,13 @@
             <a:gradFill>
               <a:gsLst>
                 <a:gs pos="0">
-                  <a:schemeClr val="accent5"/>
+                  <a:schemeClr val="accent5">
+                    <a:shade val="76000"/>
+                  </a:schemeClr>
                 </a:gs>
                 <a:gs pos="100000">
                   <a:schemeClr val="accent5">
+                    <a:shade val="76000"/>
                     <a:lumMod val="84000"/>
                   </a:schemeClr>
                 </a:gs>
@@ -348,8 +307,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.5202413879808901E-2"/>
-                  <c:y val="-1.821963394342762E-2"/>
+                  <c:x val="-1.6715598630344854E-3"/>
+                  <c:y val="5.0163539005639739E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="outEnd"/>
@@ -370,8 +329,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-7.0404827759617802E-2"/>
-                  <c:y val="-9.3094841930116468E-2"/>
+                  <c:x val="-4.9869698029306395E-3"/>
+                  <c:y val="9.74724810142652E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="outEnd"/>
@@ -385,50 +344,6 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-17E0-4CEF-A77E-4E94F824F699}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.10895985248512279"/>
-                  <c:y val="-0.13746533555185811"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="outEnd"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000002-17E0-4CEF-A77E-4E94F824F699}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.14919118263347583"/>
-                  <c:y val="-0.22066001109262345"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="outEnd"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-17E0-4CEF-A77E-4E94F824F699}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -487,101 +402,41 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'MANUFACTURING OUTPUT'!$B$4:$B$27</c:f>
+              <c:f>'MANUFACTURING OUTPUT'!$B$4:$B$10</c:f>
               <c:strCache>
-                <c:ptCount val="24"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>GPU No Shuffling</c:v>
+                  <c:v>hiddenLayer_1_Nodes_250_LearningRate_10_3_Shuffle_False</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>GPU With Shuffling</c:v>
+                  <c:v>HiddenLayer_1_Nodes_250_LearningRate_10_3_Suffling_True</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CPU No Shuffling</c:v>
+                  <c:v>HiddenLayer_1_Nodes_450_LearningRate_10_3_Shuffle_True</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CPU With Shuffling</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5/24/2017</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5/25/2017</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5/26/2017</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5/27/2017</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5/28/2017</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5/29/2017</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5/30/2017</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5/31/2017</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6/1/2017</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>6/2/2017</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>6/3/2017</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>6/4/2017</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>6/5/2017</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>6/6/2017</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>6/7/2017</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>6/8/2017</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>6/9/2017</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>6/10/2017</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>6/11/2017</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>6/12/2017</c:v>
+                  <c:v>HiddenLayer_1_Nodes_450_LearningRate_10_3_ShuffleTrue_OneSet</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'MANUFACTURING OUTPUT'!$C$4:$C$27</c:f>
+              <c:f>'MANUFACTURING OUTPUT'!$C$4:$C$10</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>17.254563999999998</c:v>
+                  <c:v>0.17293254999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.456422999999999</c:v>
+                  <c:v>0.1560917</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.293254999999998</c:v>
+                  <c:v>0.15275681999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.609170000000001</c:v>
+                  <c:v>0.12871489999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -589,6 +444,147 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-01AB-496F-ACDD-F58747B8C0B7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'MANUFACTURING OUTPUT'!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Change</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:tint val="77000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:tint val="77000"/>
+                    <a:lumMod val="84000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="1"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="76200" dir="18900000" sy="23000" kx="-1200000" algn="bl" rotWithShape="0">
+                <a:prstClr val="black">
+                  <a:alpha val="20000"/>
+                </a:prstClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'MANUFACTURING OUTPUT'!$B$4:$B$10</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>hiddenLayer_1_Nodes_250_LearningRate_10_3_Shuffle_False</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>HiddenLayer_1_Nodes_250_LearningRate_10_3_Suffling_True</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>HiddenLayer_1_Nodes_450_LearningRate_10_3_Shuffle_True</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>HiddenLayer_1_Nodes_450_LearningRate_10_3_ShuffleTrue_OneSet</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'MANUFACTURING OUTPUT'!$D$4:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-57D7-4154-A3DC-34E9166D8F36}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -658,7 +654,7 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1304,14 +1300,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>421342</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>3815715</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>460</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>142876</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1342,13 +1338,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Data" displayName="Data" ref="B3:C27" totalsRowShown="0" headerRowCellStyle="Heading 1">
-  <autoFilter ref="B3:C27"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Data" displayName="Data" ref="B3:D10" totalsRowShown="0" headerRowCellStyle="Heading 1">
+  <autoFilter ref="B3:D10"/>
+  <tableColumns count="3">
     <tableColumn id="1" name="Date" dataCellStyle="Date">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" name="Lowest Validation Error"/>
+    <tableColumn id="3" name="Change"/>
   </tableColumns>
   <tableStyleInfo name="Manufacturing Output" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1590,209 +1587,133 @@
     <tabColor theme="5"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:C27"/>
+  <dimension ref="B1:D20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="22.44140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="2.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="60.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.44140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="55.6640625" style="3" customWidth="1"/>
     <col min="7" max="7" width="2.6640625" style="3" customWidth="1"/>
     <col min="8" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:4" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:3" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.17293254999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.1560917</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.15275681999999999</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
-        <v>2</v>
+      <c r="C7" s="6">
+        <v>0.12871489999999999</v>
       </c>
-      <c r="C4" s="5">
-        <v>17.254563999999998</v>
+      <c r="D7" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="5">
-        <v>15.456422999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="5">
-        <v>17.293254999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="5">
-        <v>15.609170000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="4">
-        <f ca="1">TODAY()+4</f>
-        <v>42879</v>
-      </c>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="4"/>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="4">
-        <f ca="1">TODAY()+5</f>
-        <v>42880</v>
-      </c>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="4"/>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="4">
-        <f ca="1">TODAY()+6</f>
-        <v>42881</v>
-      </c>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="4"/>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B11" s="4">
-        <f ca="1">TODAY()+7</f>
-        <v>42882</v>
-      </c>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="4"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B12" s="4">
-        <f ca="1">TODAY()+8</f>
-        <v>42883</v>
-      </c>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="4"/>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B13" s="4">
-        <f ca="1">TODAY()+9</f>
-        <v>42884</v>
-      </c>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="4"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B14" s="4">
-        <f ca="1">TODAY()+10</f>
-        <v>42885</v>
-      </c>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="4"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B15" s="4">
-        <f ca="1">TODAY()+11</f>
-        <v>42886</v>
-      </c>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="4"/>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B16" s="4">
-        <f ca="1">TODAY()+12</f>
-        <v>42887</v>
-      </c>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="4"/>
       <c r="C16" s="5"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="4">
-        <f ca="1">TODAY()+13</f>
-        <v>42888</v>
-      </c>
+      <c r="B17" s="4"/>
       <c r="C17" s="5"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="4">
-        <f ca="1">TODAY()+14</f>
-        <v>42889</v>
-      </c>
+      <c r="B18" s="4"/>
       <c r="C18" s="5"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" s="4">
-        <f ca="1">TODAY()+15</f>
-        <v>42890</v>
-      </c>
+      <c r="B19" s="4"/>
       <c r="C19" s="5"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B20" s="4">
-        <f ca="1">TODAY()+16</f>
-        <v>42891</v>
-      </c>
+      <c r="B20" s="4"/>
       <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B21" s="4">
-        <f ca="1">TODAY()+17</f>
-        <v>42892</v>
-      </c>
-      <c r="C21" s="5"/>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B22" s="4">
-        <f ca="1">TODAY()+18</f>
-        <v>42893</v>
-      </c>
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B23" s="4">
-        <f ca="1">TODAY()+19</f>
-        <v>42894</v>
-      </c>
-      <c r="C23" s="5"/>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B24" s="4">
-        <f ca="1">TODAY()+20</f>
-        <v>42895</v>
-      </c>
-      <c r="C24" s="5"/>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B25" s="4">
-        <f ca="1">TODAY()+21</f>
-        <v>42896</v>
-      </c>
-      <c r="C25" s="5"/>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B26" s="4">
-        <f ca="1">TODAY()+22</f>
-        <v>42897</v>
-      </c>
-      <c r="C26" s="5"/>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B27" s="4">
-        <f ca="1">TODAY()+23</f>
-        <v>42898</v>
-      </c>
-      <c r="C27" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="5">
@@ -1808,9 +1729,6 @@
   <headerFooter differentFirst="1">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
-  <ignoredErrors>
-    <ignoredError sqref="B8:B27" calculatedColumn="1"/>
-  </ignoredErrors>
   <drawing r:id="rId2"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>

</xml_diff>

<commit_message>
change name of the columns
</commit_message>
<xml_diff>
--- a/Processor/Manufacturing output chart1.xlsx
+++ b/Processor/Manufacturing output chart1.xlsx
@@ -15,7 +15,7 @@
     <sheet name="MANUFACTURING OUTPUT" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ColumnTitle1">Data[[#Headers],[Date]]</definedName>
+    <definedName name="ColumnTitle1">Data[[#Headers],[Trials]]</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'MANUFACTURING OUTPUT'!$3:$3</definedName>
   </definedNames>
   <calcPr calcId="171027" concurrentCalc="0"/>
@@ -30,28 +30,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Manufacturing Output Data</t>
-  </si>
-  <si>
-    <t>Lowest Validation Error</t>
-  </si>
-  <si>
-    <t>HiddenLayer_1_Nodes_450_LearningRate_10_3_Shuffle_True</t>
-  </si>
-  <si>
-    <t>HiddenLayer_1_Nodes_450_LearningRate_10_3_ShuffleTrue_OneSet</t>
-  </si>
-  <si>
     <t>hiddenLayer_1_Nodes_250_LearningRate_10_3_Shuffle_False</t>
   </si>
   <si>
     <t>shuffling</t>
-  </si>
-  <si>
-    <t>HiddenLayer_1_Nodes_250_LearningRate_10_3_Suffling_True</t>
   </si>
   <si>
     <t>inc nodes</t>
@@ -62,12 +44,79 @@
   <si>
     <t>Change</t>
   </si>
+  <si>
+    <t>Summary Of Results</t>
+  </si>
+  <si>
+    <t>Trials</t>
+  </si>
+  <si>
+    <t>DER</t>
+  </si>
+  <si>
+    <r>
+      <t>HiddenLayer_1_Nodes_250_LearningRate_10_3_Suffling_</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="3" tint="-0.24994659260841701"/>
+        <rFont val="Corbel"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>True</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>HiddenLayer_1_Nodes_</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="3" tint="-0.24994659260841701"/>
+        <rFont val="Corbel"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>450</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="3" tint="-0.24994659260841701"/>
+        <rFont val="Corbel"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_LearningRate_10_3_Shuffle_True</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>HiddenLayer_1_Nodes_450_LearningRate_10_3_ShuffleTrue_</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="3" tint="-0.24994659260841701"/>
+        <rFont val="Corbel"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OneSet</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="3" tint="-0.24994659260841701"/>
@@ -103,6 +152,14 @@
       <name val="Trebuchet MS"/>
       <family val="2"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3" tint="-0.24994659260841701"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -158,7 +215,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -173,7 +230,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -268,7 +331,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Lowest Validation Error</c:v>
+                  <c:v>DER</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1341,10 +1404,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Data" displayName="Data" ref="B3:D10" totalsRowShown="0" headerRowCellStyle="Heading 1">
   <autoFilter ref="B3:D10"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Date" dataCellStyle="Date">
+    <tableColumn id="1" name="Trials" dataCellStyle="Date">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Lowest Validation Error"/>
+    <tableColumn id="2" name="DER"/>
     <tableColumn id="3" name="Change"/>
   </tableColumns>
   <tableStyleInfo name="Manufacturing Output" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1590,7 +1653,7 @@
   <dimension ref="B1:D20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1606,61 +1669,61 @@
   <sheetData>
     <row r="1" spans="2:4" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="1" t="s">
-        <v>0</v>
+      <c r="B3" s="6" t="s">
+        <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
+      <c r="C3" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
-        <v>5</v>
+      <c r="B4" s="7" t="s">
+        <v>0</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="8">
         <v>0.17293254999999999</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="4" t="s">
-        <v>7</v>
+      <c r="B5" s="7" t="s">
+        <v>8</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="8">
         <v>0.1560917</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="4" t="s">
-        <v>3</v>
+      <c r="B6" s="7" t="s">
+        <v>9</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="8">
         <v>0.15275681999999999</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="4" t="s">
-        <v>4</v>
+      <c r="B7" s="7" t="s">
+        <v>10</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="8">
         <v>0.12871489999999999</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Copy Results Of Other Laptop
</commit_message>
<xml_diff>
--- a/Processor/Manufacturing output chart1.xlsx
+++ b/Processor/Manufacturing output chart1.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>shuffling</t>
   </si>
@@ -141,70 +141,9 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>HiddenLayer_1_Nodes_450_LearningRate_10_3_ShuffleTrue_</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="3" tint="-0.24994659260841701"/>
-        <rFont val="Corbel"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Same_ValidationSet_QuranKarim</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>HiddenLayer_1_Nodes_</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="3" tint="-0.24994659260841701"/>
-        <rFont val="Corbel"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>450</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="3" tint="-0.24994659260841701"/>
-        <rFont val="Corbel"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_LearningRate_10_3_Shuffle_True_QuranKarim</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>HiddenLayer_1_Nodes_250_LearningRate_10_3_Suffling_</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="3" tint="-0.24994659260841701"/>
-        <rFont val="Corbel"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>True_QuranKarim</t>
-    </r>
-  </si>
-  <si>
     <t>hiddenLayer_1_Nodes_250_LearningRate_10_3_Shuffle_False_QuranKarim</t>
   </si>
   <si>
-    <t>2-new techniques 450 nodes same validation 10_3</t>
-  </si>
-  <si>
     <t>HiddenLayer_1_Nodes_450_LearningRate_10_3_Shuffle_True_NewTechniques_QuranKarim</t>
   </si>
   <si>
@@ -212,13 +151,34 @@
   </si>
   <si>
     <t>HiddenLayer_1_Nodes_150_LearningRate_10_3_ShuffleTrue_NewTechnique_QuranKarim</t>
+  </si>
+  <si>
+    <t>HiddenLayer_1_Nodes_350_Shuffle_True_LearningRate_10_3_QuranKarim</t>
+  </si>
+  <si>
+    <t>HiddenLayer_1_Nodes_350_Shuffle_True_CPU_70TrainingSet_30TestingSet_NoValidationSet_QuranKarim</t>
+  </si>
+  <si>
+    <t>HiddenLayer_1_Nodes_450_LearningRate_10_3_Shuffle_True_QuranKarim</t>
+  </si>
+  <si>
+    <t>HiddenLayer_1_Nodes_250_LearningRate_10_3_Suffling_True_QuranKarim</t>
+  </si>
+  <si>
+    <t>HiddenLayer_1_Nodes_450_LearningRate_10_3_ShuffleTrue_Same_ValidationSet_QuranKarim</t>
+  </si>
+  <si>
+    <t>HiddenLayer_1_Nodes_450_LearnigRate_10_3_Shuffle_True_NewTechnique_SameValidationSet_QuranKarim</t>
+  </si>
+  <si>
+    <t>HiddenLayer_1_Nodes_450_LearningRate_10_5_Shuffle_True_NewTechnique_SameValidationSet_QuranKarim</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="3" tint="-0.24994659260841701"/>
@@ -263,6 +223,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -289,7 +255,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -303,6 +269,19 @@
       <top/>
       <bottom style="medium">
         <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom style="thin">
+        <color theme="8"/>
       </bottom>
       <diagonal/>
     </border>
@@ -323,7 +302,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -332,9 +311,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="right"/>
     </xf>
@@ -347,15 +323,8 @@
     <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="10" fontId="5" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1">
       <alignment horizontal="right"/>
@@ -363,6 +332,19 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Components" xfId="5"/>
@@ -589,9 +571,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'MANUFACTURING OUTPUT'!$B$4:$B$21</c:f>
+              <c:f>'MANUFACTURING OUTPUT'!$B$4:$B$30</c:f>
               <c:strCache>
-                <c:ptCount val="18"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>hiddenLayer_1_Nodes_250_LearningRate_10_3_Shuffle_False_QuranKarim</c:v>
                 </c:pt>
@@ -602,39 +584,48 @@
                   <c:v>HiddenLayer_1_Nodes_450_LearningRate_10_3_Shuffle_True_QuranKarim</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>HiddenLayer_1_Nodes_350_Shuffle_True_LearningRate_10_3_QuranKarim</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>HiddenLayer_1_Nodes_350_Shuffle_True_CPU_70TrainingSet_30TestingSet_NoValidationSet_QuranKarim</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>HiddenLayer_1_Nodes_450_LearningRate_10_3_ShuffleTrue_Same_ValidationSet_QuranKarim</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
+                  <c:v>HiddenLayer_1_Nodes_150_LearningRate_10_3_ShuffleTrue_NewTechnique_QuranKarim</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>HiddenLayer_1_Nodes_250_LearningRate_10_3_Shuffle_True_NewTechnique_QuranKarim</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>HiddenLayer_1_Nodes_450_LearningRate_10_3_Shuffle_True_NewTechniques_QuranKarim</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>HiddelLayer_1_Nodes_250_LearningRate_10_5_Shuffle_True_NewTechnique_QuranKarim</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>HiddenLayer_1_Nodes_250_LearningRate_10_3_Shuffle_True_NewTechnique_QuranKarim</c:v>
-                </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
+                  <c:v>HiddenLayer_1_Nodes_450_LearningRate_10_5_Shuffle_True_NewTechniques_QuranKarim</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>HiddenLayer_1_Nodes_250_LearningRate_10_3_Shuffle_True_NewTechnique_Same_ValidationSet_QuranKarim</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>HiddenLayer_1_Nodes_450_LearningRate_10_3_Shuffle_True_NewTechniques_QuranKarim</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>HiddenLayer_1_Nodes_450_LearningRate_10_5_Shuffle_True_NewTechniques_QuranKarim</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>HiddenLayer_1_Nodes_150_LearningRate_10_3_ShuffleTrue_NewTechnique_QuranKarim</c:v>
-                </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
+                  <c:v>HiddenLayer_1_Nodes_450_LearningRate_10_5_Shuffle_True_NewTechnique_SameValidationSet_QuranKarim</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>HiddenLayer_1_Nodes_450_LearnigRate_10_3_Shuffle_True_NewTechnique_SameValidationSet_QuranKarim</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>0- check in other papers what part of each document is taken for trainig and testing</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>2-new techniques 450 nodes same validation 10_3</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="24">
                   <c:v>4-new techniques 150 nodes same validation</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="25">
                   <c:v>5-try feed forward for best result</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="26">
                   <c:v>6- check how we you will implement post processing</c:v>
                 </c:pt>
               </c:strCache>
@@ -642,10 +633,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'MANUFACTURING OUTPUT'!$C$4:$C$21</c:f>
+              <c:f>'MANUFACTURING OUTPUT'!$C$4:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0.17293254999999999</c:v>
                 </c:pt>
@@ -656,25 +647,37 @@
                   <c:v>0.15275681999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>9.7000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1069</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0.12871489999999999</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
+                  <c:v>0.14050000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1033</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1071</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0.1303</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.1033</c:v>
-                </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
+                  <c:v>0.14030000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>0.14430000000000001</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.1071</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.14030000000000001</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.14050000000000001</c:v>
+                <c:pt idx="14">
+                  <c:v>0.17449999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.13450000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -784,9 +787,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'MANUFACTURING OUTPUT'!$B$4:$B$21</c:f>
+              <c:f>'MANUFACTURING OUTPUT'!$B$4:$B$30</c:f>
               <c:strCache>
-                <c:ptCount val="18"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>hiddenLayer_1_Nodes_250_LearningRate_10_3_Shuffle_False_QuranKarim</c:v>
                 </c:pt>
@@ -797,39 +800,48 @@
                   <c:v>HiddenLayer_1_Nodes_450_LearningRate_10_3_Shuffle_True_QuranKarim</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>HiddenLayer_1_Nodes_350_Shuffle_True_LearningRate_10_3_QuranKarim</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>HiddenLayer_1_Nodes_350_Shuffle_True_CPU_70TrainingSet_30TestingSet_NoValidationSet_QuranKarim</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>HiddenLayer_1_Nodes_450_LearningRate_10_3_ShuffleTrue_Same_ValidationSet_QuranKarim</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
+                  <c:v>HiddenLayer_1_Nodes_150_LearningRate_10_3_ShuffleTrue_NewTechnique_QuranKarim</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>HiddenLayer_1_Nodes_250_LearningRate_10_3_Shuffle_True_NewTechnique_QuranKarim</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>HiddenLayer_1_Nodes_450_LearningRate_10_3_Shuffle_True_NewTechniques_QuranKarim</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>HiddelLayer_1_Nodes_250_LearningRate_10_5_Shuffle_True_NewTechnique_QuranKarim</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>HiddenLayer_1_Nodes_250_LearningRate_10_3_Shuffle_True_NewTechnique_QuranKarim</c:v>
-                </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
+                  <c:v>HiddenLayer_1_Nodes_450_LearningRate_10_5_Shuffle_True_NewTechniques_QuranKarim</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>HiddenLayer_1_Nodes_250_LearningRate_10_3_Shuffle_True_NewTechnique_Same_ValidationSet_QuranKarim</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>HiddenLayer_1_Nodes_450_LearningRate_10_3_Shuffle_True_NewTechniques_QuranKarim</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>HiddenLayer_1_Nodes_450_LearningRate_10_5_Shuffle_True_NewTechniques_QuranKarim</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>HiddenLayer_1_Nodes_150_LearningRate_10_3_ShuffleTrue_NewTechnique_QuranKarim</c:v>
-                </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
+                  <c:v>HiddenLayer_1_Nodes_450_LearningRate_10_5_Shuffle_True_NewTechnique_SameValidationSet_QuranKarim</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>HiddenLayer_1_Nodes_450_LearnigRate_10_3_Shuffle_True_NewTechnique_SameValidationSet_QuranKarim</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>0- check in other papers what part of each document is taken for trainig and testing</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>2-new techniques 450 nodes same validation 10_3</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="24">
                   <c:v>4-new techniques 150 nodes same validation</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="25">
                   <c:v>5-try feed forward for best result</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="26">
                   <c:v>6- check how we you will implement post processing</c:v>
                 </c:pt>
               </c:strCache>
@@ -837,17 +849,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'MANUFACTURING OUTPUT'!$D$4:$D$21</c:f>
+              <c:f>'MANUFACTURING OUTPUT'!$D$4:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1609,8 +1621,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Data" displayName="Data" ref="B3:D21" totalsRowShown="0" headerRowCellStyle="Heading 1">
-  <autoFilter ref="B3:D21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Data" displayName="Data" ref="B3:D23" totalsRowShown="0" headerRowCellStyle="Heading 1">
+  <autoFilter ref="B3:D23"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Trials" dataCellStyle="Date">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
@@ -1858,10 +1870,10 @@
     <tabColor theme="5"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:D21"/>
+  <dimension ref="B1:D30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1883,10 +1895,10 @@
     </row>
     <row r="2" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:4" ht="35.1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1894,18 +1906,18 @@
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="8">
+      <c r="B4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="7">
         <v>0.17293254999999999</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="8">
+      <c r="B5" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="7">
         <v>0.1560917</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -1913,10 +1925,10 @@
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="8">
+      <c r="B6" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="7">
         <v>0.15275681999999999</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -1924,106 +1936,142 @@
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="7" t="s">
-        <v>14</v>
+      <c r="B7" s="17" t="s">
+        <v>18</v>
       </c>
       <c r="C7" s="8">
+        <v>9.7000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0.1069</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="7">
         <v>0.12871489999999999</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="4"/>
-      <c r="C8" s="8"/>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="7" t="s">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="14"/>
+      <c r="C10" s="16"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0.14050000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0.1033</v>
+      </c>
+      <c r="D12" s="15"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0.1071</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C14" s="7">
         <v>0.1303</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="10">
-        <v>0.1033</v>
-      </c>
-      <c r="D10" s="11"/>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="7" t="s">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0.14030000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="9"/>
+      <c r="C16" s="16"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C17" s="7">
         <v>0.14430000000000001</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="8">
-        <v>0.1071</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="8">
-        <v>0.14030000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="8">
-        <v>0.14050000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="13"/>
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B16" s="13"/>
-      <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="4" t="s">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="7">
+        <v>0.17449999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="7">
+        <v>0.13450000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="9"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="9"/>
+      <c r="C21" s="4"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="9"/>
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" s="9"/>
+      <c r="C23" s="4"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" s="4" t="s">
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27" s="12"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B28" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B20" s="4" t="s">
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B29" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B21" s="4" t="s">
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="5">

</xml_diff>